<commit_message>
add PR-AUC and ROC-AUC
</commit_message>
<xml_diff>
--- a/Models_results_resume.xlsx
+++ b/Models_results_resume.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\Documents\Data_Analytics_Ironhack\Projects\google_brain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1635C159-7022-4A27-BD39-278FF5B288AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE856802-BABF-429F-969C-78F566F5BF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{6E426249-09DC-4440-91B9-0D30DCF95C62}"/>
+    <workbookView xWindow="-38505" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{6E426249-09DC-4440-91B9-0D30DCF95C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t>Model</t>
   </si>
@@ -72,13 +73,31 @@
   </si>
   <si>
     <t>Balanced</t>
+  </si>
+  <si>
+    <t>w/ Class weight</t>
+  </si>
+  <si>
+    <t>w/ SMOTE</t>
+  </si>
+  <si>
+    <t>w/ oversampling</t>
+  </si>
+  <si>
+    <t>w/ undersampling</t>
+  </si>
+  <si>
+    <t>ROC-AUC</t>
+  </si>
+  <si>
+    <t>PR-AUC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,16 +113,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -126,11 +159,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -142,9 +188,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -162,6 +224,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CBD701F-B000-2860-FE10-79DBF05C0D0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1838325" y="7629525"/>
+          <a:ext cx="8058150" cy="3990975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A5C6FC-089E-499B-816D-03EF35F4F785}">
   <dimension ref="A2:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,75 +627,75 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -599,7 +727,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2">
@@ -631,7 +759,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2">
@@ -674,4 +802,549 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EB0086-FA5A-43D8-8DAB-947B3F17F7EC}">
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.87</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.87</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.61</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.437</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.47</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.19</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9">
+        <v>0.59</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.41</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.83</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.37</v>
+      </c>
+      <c r="L6" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9">
+        <v>0.41</v>
+      </c>
+      <c r="O6" s="9">
+        <v>0.46</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.87</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0.68</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.41</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.37</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.87</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.61</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.19</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.49</v>
+      </c>
+      <c r="D20" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.437</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0.83</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.88700000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>